<commit_message>
Added color coding to denote which items have been added to the database
</commit_message>
<xml_diff>
--- a/PlantsDatabaseItems.xlsx
+++ b/PlantsDatabaseItems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertsd11\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creemb\AndroidStudioProjects\PartyThyme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566682E-1305-4D0B-944F-76DE9587F767}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECB469-111B-462E-91BF-F0E68B6BBE66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F084FB0F-668D-4AED-9839-88C98B8F3DAC}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Low Maintenance</t>
-  </si>
-  <si>
-    <t>Med Maintenance</t>
-  </si>
-  <si>
-    <t>High Maintenance</t>
-  </si>
-  <si>
     <t>Flowering</t>
   </si>
   <si>
@@ -315,6 +306,27 @@
   </si>
   <si>
     <t>Purple</t>
+  </si>
+  <si>
+    <t>Maintenance (1-3)</t>
+  </si>
+  <si>
+    <t>Prune canes of older plants to control height</t>
+  </si>
+  <si>
+    <t>Every 2 weeks in spring and summer with a balanced furtilizer. Reduce to once a month during fall and none during winter</t>
+  </si>
+  <si>
+    <t>Bright, filtered light such as through a curtain in front of a sunny window)</t>
+  </si>
+  <si>
+    <t>6.5 to 7.5</t>
+  </si>
+  <si>
+    <t>Keep soil moist but never soggy</t>
+  </si>
+  <si>
+    <t>Well-draining</t>
   </si>
 </sst>
 </file>
@@ -670,7 +682,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,18 +691,22 @@
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" customWidth="1"/>
-    <col min="22" max="23" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="111.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="21" width="7.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" customWidth="1"/>
     <col min="25" max="25" width="16.5703125" customWidth="1"/>
   </cols>
@@ -703,10 +719,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -715,66 +731,60 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="S1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" t="s">
-        <v>10</v>
-      </c>
       <c r="W1" t="s">
-        <v>52</v>
-      </c>
-      <c r="X1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -789,40 +799,40 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -834,24 +844,18 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -866,40 +870,40 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>6.5</v>
+      </c>
+      <c r="N3" t="s">
         <v>64</v>
       </c>
-      <c r="M3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
       <c r="O3">
-        <v>6.5</v>
-      </c>
-      <c r="P3" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -914,21 +918,16 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -943,31 +942,40 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" t="s">
         <v>69</v>
       </c>
-      <c r="J4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" t="s">
-        <v>71</v>
-      </c>
-      <c r="P4" t="s">
-        <v>72</v>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -982,21 +990,15 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>68</v>
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1011,12 +1013,63 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1031,12 +1084,15 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1051,12 +1107,15 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1071,12 +1130,15 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1091,12 +1153,15 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1111,12 +1176,15 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1131,32 +1199,38 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1171,12 +1245,15 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1191,12 +1268,15 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1211,277 +1291,319 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>89</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>94</v>
+      <c r="G28">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished gathering data for database
</commit_message>
<xml_diff>
--- a/PlantsDatabaseItems.xlsx
+++ b/PlantsDatabaseItems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creemb\AndroidStudioProjects\PartyThyme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECB469-111B-462E-91BF-F0E68B6BBE66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46BD867-C61A-43B7-BFD8-47DEDDEE67A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F084FB0F-668D-4AED-9839-88C98B8F3DAC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F084FB0F-668D-4AED-9839-88C98B8F3DAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="214">
   <si>
     <t>Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>PHMaintain</t>
   </si>
   <si>
-    <t>FruitVegetable</t>
-  </si>
-  <si>
     <t>Poisionous</t>
   </si>
   <si>
@@ -327,6 +324,354 @@
   </si>
   <si>
     <t>Well-draining</t>
+  </si>
+  <si>
+    <t>Wait for the plant to droop slightly before watering. In general, water at least once a week and keep the soil moist</t>
+  </si>
+  <si>
+    <t>Partial shade, can tolerate fluorescent lights. Yellow leaves show light too strong, brown indicate scorching</t>
+  </si>
+  <si>
+    <t>6.5 to 7.6</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>10 to 11</t>
+  </si>
+  <si>
+    <t>Keep the soil moist</t>
+  </si>
+  <si>
+    <t>None needed</t>
+  </si>
+  <si>
+    <t>High humidity, indirect light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil should remain damp. In general water once a day, mist once or twice a week. </t>
+  </si>
+  <si>
+    <t>Plant with peat moss and keep moss hydrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fertilizer should only be given to the plant a few times a year. </t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Does well in dry soil or in vases of water. Very flexible</t>
+  </si>
+  <si>
+    <t>Thrive in both nutirent rich and poor soil</t>
+  </si>
+  <si>
+    <t>Bright indirect light. Do not do well in direct sunlight</t>
+  </si>
+  <si>
+    <t>Fertilize every 1 to 3 months to grow quicker, but none necessary</t>
+  </si>
+  <si>
+    <t>Cuttings can be taken from a mother plant and rooted in water for a house plant</t>
+  </si>
+  <si>
+    <t>Fast draining sandy soil</t>
+  </si>
+  <si>
+    <t>Soil should dry between waterings. During winter reduce to watering monthly. Underwatering is better. Too much will kill plant</t>
+  </si>
+  <si>
+    <t>Feed with mild cactus fertilizer during growing sesaon or balanced slow-release (10-10-10) fertilizer. Do not fertilize in winter</t>
+  </si>
+  <si>
+    <t>Indirect but steady light with some direct sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow top 1/3 of soil to dry before watering. Barely moist but never soggy. Do not allow to sit in excess water that drains from pot. </t>
+  </si>
+  <si>
+    <t>Basic well-aerated potting soil that drains quicly but retains water</t>
+  </si>
+  <si>
+    <t>Feed montly in spring and summer with a fertlizer high in nitrogen at 1/2 the recommended strength. Do not use if plant is dry or not growing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bright indirect light </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bright indirect light  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown leaf tips should be cut off with wet scissors. Bare stalks should be removed. </t>
+  </si>
+  <si>
+    <t>During growing season it needs to be kept moist. Wipe leaves with damp cloth or spritz with water. During dormant season may only need water once or twice a month</t>
+  </si>
+  <si>
+    <t>General potting soil in large pot</t>
+  </si>
+  <si>
+    <t>Bright indirect light that isn't too hot.</t>
+  </si>
+  <si>
+    <t>Cut a sllit in nodes where leaves fall off to allow new leaves to grow quicker</t>
+  </si>
+  <si>
+    <t>Does best in dry conditions. Should be allowed to go completely dry before watering. When watered, soil should be drenched but allowed to drain</t>
+  </si>
+  <si>
+    <t>Cactus potting soil mix with perlite or building sand</t>
+  </si>
+  <si>
+    <t>Need bright light. Best in south  or west facing windows</t>
+  </si>
+  <si>
+    <t>Edible</t>
+  </si>
+  <si>
+    <t>Water deeply but allow to dry out completely before you give more moisture</t>
+  </si>
+  <si>
+    <t>60 percent peat moss 40 percent perlite</t>
+  </si>
+  <si>
+    <t>Fertilize once a month during growing season with a houseplant food</t>
+  </si>
+  <si>
+    <t>Partial sun to light shade areas. Strong sun can burn tips of leaves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take a 2 to 3 inch section and strip off the bottom leaves. </t>
+  </si>
+  <si>
+    <t>Likes humidity but should let soil dry out between watering. Water thoroughly until water flows out of drainage hole of pot</t>
+  </si>
+  <si>
+    <t>Peat-moss based soil in pot with good drainage</t>
+  </si>
+  <si>
+    <t>During growing season fertilize once a month with a liquid plant food at half strength. No fertilizer in winter</t>
+  </si>
+  <si>
+    <t>Bright indirect light with moderate to high humidity</t>
+  </si>
+  <si>
+    <t>Can do well in low light but prefer bright indirect light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cut off the tip of a stem with at least two leaf nodes. </t>
+  </si>
+  <si>
+    <t>Check soil before watering. Prefers to be slightly on dry side. Make sure it has excellent drainage</t>
+  </si>
+  <si>
+    <t>Well-drained soil. Best in average loams</t>
+  </si>
+  <si>
+    <t>Feed every 2 weeks during spring and summer with half recommended dose. Fertilize monthly in fall and winter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial shade to full shade. </t>
+  </si>
+  <si>
+    <t>Partial shade to full shade</t>
+  </si>
+  <si>
+    <t>Wide range</t>
+  </si>
+  <si>
+    <t>Trim ground cover in spring to keep manageable and prevent bacteria</t>
+  </si>
+  <si>
+    <t>4 to 9</t>
+  </si>
+  <si>
+    <t>Moderate watering, allow plant to dry some before watering. Overwatering will lead to root rot</t>
+  </si>
+  <si>
+    <t>Well-draining equal mix of potting soil, perlite and sand</t>
+  </si>
+  <si>
+    <t>Fertilize older plants once or twice yearly using a water-soluable houseplant fertilizer</t>
+  </si>
+  <si>
+    <t>Medium to low light, or indirect sunlight</t>
+  </si>
+  <si>
+    <t>Can give the plant a trim if it gets too big. Most people cut flowers prior to seed production</t>
+  </si>
+  <si>
+    <t>6 to 9</t>
+  </si>
+  <si>
+    <t>Keep soil lightly moist spring through fall. Allow surface to dry between waterings in winter</t>
+  </si>
+  <si>
+    <t>Peat-moss based mix such as African violet</t>
+  </si>
+  <si>
+    <t>Feed monthly spring through fall with a balanced liquid fertilizer diluted by half</t>
+  </si>
+  <si>
+    <t>Moderate to bright light. Small leaves indicate not enough light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No direct sun. Moderate to bright light. </t>
+  </si>
+  <si>
+    <t>Take stem tip cuttings in spring or early summer. Roots easily in water or moist soil</t>
+  </si>
+  <si>
+    <t>Water enough to keep soil lightly moist in spring and summer and allow soil to dry between waterings in fall and winter</t>
+  </si>
+  <si>
+    <t>Fertilize with a time release fertilizer in spring. Can use a liquid houseplant fertilizer that contains micronutrients for this. Do not feed in fall or winter</t>
+  </si>
+  <si>
+    <t>Bright indirect light. Leaves turn yellow in direct sunlight</t>
+  </si>
+  <si>
+    <t>Bright indirect light</t>
+  </si>
+  <si>
+    <t>Can tolerate trimming without serious harm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overwatering can be a problem. Keep soil moist but not soggy. Check to make sure it is dry 1 inch down before watering </t>
+  </si>
+  <si>
+    <t>When growing, fertilize twice a month to encourage growth. A houseplant food high in nitrogen can be applied at half strength</t>
+  </si>
+  <si>
+    <t>Filtered light, such as through a sheer curtain or other window cover</t>
+  </si>
+  <si>
+    <t>Water sparingly and allow to dry as deep as 5 inches between waterings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General potting soil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fertilize occassionally with a balanced houseplant food after watering. Leach in summer by flushing with water to remove salts </t>
+  </si>
+  <si>
+    <t>Medium to low light away from direct sun</t>
+  </si>
+  <si>
+    <t>Can use fluorescent lighting</t>
+  </si>
+  <si>
+    <t>Water only when soil is dry to the touch. Water thoroughly and allow to dry out again. Brown leaves on bottom indicate overwatering, brown leaves elsewhere show underwatering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich well-draining peaty soil. </t>
+  </si>
+  <si>
+    <t>Feed with a water-soluable plant food throughout the growing season</t>
+  </si>
+  <si>
+    <t>Bright consistent light preferably by a sunny window. Turn every few months</t>
+  </si>
+  <si>
+    <t>Crown should be visible and allowed to dry between watering. Water in morning so leaves can dry during day to lessen risk of fungal diseases</t>
+  </si>
+  <si>
+    <t>Sandy soil with a little compost added at planting</t>
+  </si>
+  <si>
+    <t>Can be enhanced witth a micro-nutrient liquid fertilizer such as a seaweed or fish emulsion, but is not necssary</t>
+  </si>
+  <si>
+    <t>Bright, indirect light</t>
+  </si>
+  <si>
+    <t>Loamy soil</t>
+  </si>
+  <si>
+    <t>4.5 to 6.5</t>
+  </si>
+  <si>
+    <t>Fertilize in spring with organic acid plant fertilizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In general water moderately. In spring water deeply every 2 weeks. </t>
+  </si>
+  <si>
+    <t>Partial sun or dappled sun</t>
+  </si>
+  <si>
+    <t>Partila sun or dappled sun</t>
+  </si>
+  <si>
+    <t>4 to 8</t>
+  </si>
+  <si>
+    <t>Keep soil moist but not wet</t>
+  </si>
+  <si>
+    <t>Well-draining potting mix</t>
+  </si>
+  <si>
+    <t>Balanced liquid fertilizer, monthly to biweekly as needed</t>
+  </si>
+  <si>
+    <t>Partial sun preferred, may tolerate full sun in limited conditions</t>
+  </si>
+  <si>
+    <t>Partial sun preferred</t>
+  </si>
+  <si>
+    <t>Stem cuttings can be used for propagation</t>
+  </si>
+  <si>
+    <t>Water when soil dries through the first half inch, then water thoroughly and let drain. Adult plants require less water. Don’t let sit in water</t>
+  </si>
+  <si>
+    <t>Well-draining, airy, light soil</t>
+  </si>
+  <si>
+    <t>Use liquid fertilizer weekly at quarter strength or biweekly at half strength. Every 3rd or 4th feeding use a high phosphorous fertilizer</t>
+  </si>
+  <si>
+    <t>Can grow in full sun in all but hottest climates. Give as much bright light as possible</t>
+  </si>
+  <si>
+    <t>Can propogate from leaf tip cuttings</t>
+  </si>
+  <si>
+    <t>Water regularly to keep soil evenly moist</t>
+  </si>
+  <si>
+    <t>General soil for indoor, light mulch for outdoor</t>
+  </si>
+  <si>
+    <t>Topdress plants with a thin layer of compost or organic fertilizer every few months. Above ground pots need winter protection in cold climates</t>
+  </si>
+  <si>
+    <t>Needs 6 hours minimum of direct sunlight daily</t>
+  </si>
+  <si>
+    <t>May be started indoors under fluorescent lights during winter</t>
+  </si>
+  <si>
+    <t>Benefits from picking and pruning</t>
+  </si>
+  <si>
+    <t>3 to 11</t>
+  </si>
+  <si>
+    <t>Water basic when soil is dry doing your best to water plant at base and not water the leaves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well-drained soil.  </t>
+  </si>
+  <si>
+    <t>6 hours of direct sunlight daily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can prune basil leaves for eating and propogation </t>
   </si>
 </sst>
 </file>
@@ -342,12 +687,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -362,9 +719,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE613F1F-930B-4552-950E-90474DDAC4DB}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +1052,7 @@
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="117" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="111.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="67.28515625" bestFit="1" customWidth="1"/>
@@ -719,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -731,37 +1090,37 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
         <v>43</v>
-      </c>
-      <c r="L1" t="s">
-        <v>44</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O1" t="s">
         <v>4</v>
       </c>
       <c r="P1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
       </c>
       <c r="R1" t="s">
         <v>5</v>
@@ -773,17 +1132,17 @@
         <v>7</v>
       </c>
       <c r="U1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V1" t="s">
         <v>8</v>
       </c>
       <c r="W1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -799,31 +1158,31 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
       <c r="K2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -850,12 +1209,12 @@
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -870,31 +1229,31 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>57</v>
       </c>
       <c r="M3">
         <v>6.5</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -921,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
+      <c r="A4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -942,32 +1301,32 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
         <v>66</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
         <v>67</v>
       </c>
-      <c r="K4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>68</v>
       </c>
-      <c r="N4" t="s">
-        <v>69</v>
-      </c>
       <c r="O4">
         <v>1</v>
       </c>
@@ -993,12 +1352,12 @@
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
+      <c r="A5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1013,31 +1372,31 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" t="s">
         <v>97</v>
       </c>
-      <c r="I5" t="s">
-        <v>98</v>
-      </c>
       <c r="J5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" t="s">
         <v>94</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>94</v>
+      </c>
+      <c r="M5" t="s">
         <v>95</v>
       </c>
-      <c r="L5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M5" t="s">
-        <v>96</v>
-      </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1064,12 +1423,12 @@
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
+      <c r="A6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1084,15 +1443,63 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
+      <c r="A7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1112,10 +1519,58 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" t="s">
+        <v>109</v>
+      </c>
+      <c r="N7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
+      <c r="A8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1130,15 +1585,63 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" t="s">
+        <v>114</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
+      <c r="A9" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1153,15 +1656,63 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9">
         <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" t="s">
+        <v>118</v>
+      </c>
+      <c r="L9" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9" t="s">
+        <v>109</v>
+      </c>
+      <c r="N9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
+      <c r="A10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1181,10 +1732,58 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" t="s">
+        <v>109</v>
+      </c>
+      <c r="N10" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1199,15 +1798,63 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11">
         <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" t="s">
+        <v>127</v>
+      </c>
+      <c r="M11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1222,15 +1869,63 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12">
         <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" t="s">
+        <v>131</v>
+      </c>
+      <c r="M12" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" t="s">
+        <v>101</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
+      <c r="A13" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1245,15 +1940,63 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" t="s">
+        <v>137</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
+      <c r="A14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1268,15 +2011,63 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14">
         <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" t="s">
+        <v>140</v>
+      </c>
+      <c r="K14" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" t="s">
+        <v>142</v>
+      </c>
+      <c r="M14" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" t="s">
+        <v>143</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
+      <c r="A15" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1291,153 +2082,489 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15">
         <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" t="s">
+        <v>147</v>
+      </c>
+      <c r="L15" t="s">
+        <v>148</v>
+      </c>
+      <c r="M15" t="s">
+        <v>149</v>
+      </c>
+      <c r="N15" t="s">
+        <v>150</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>152</v>
+      </c>
+      <c r="I16" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" t="s">
+        <v>155</v>
+      </c>
+      <c r="L16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M16" t="s">
+        <v>109</v>
+      </c>
+      <c r="N16" t="s">
+        <v>156</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>81</v>
       </c>
-      <c r="G16">
-        <v>1</v>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" t="s">
+        <v>161</v>
+      </c>
+      <c r="L17" t="s">
+        <v>162</v>
+      </c>
+      <c r="M17" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" t="s">
+        <v>163</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>82</v>
       </c>
-      <c r="G17">
-        <v>1</v>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" t="s">
+        <v>173</v>
+      </c>
+      <c r="J18" t="s">
+        <v>165</v>
+      </c>
+      <c r="K18" t="s">
+        <v>166</v>
+      </c>
+      <c r="L18" t="s">
+        <v>167</v>
+      </c>
+      <c r="M18" t="s">
+        <v>109</v>
+      </c>
+      <c r="N18" t="s">
+        <v>168</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>83</v>
       </c>
-      <c r="G18">
-        <v>1</v>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>169</v>
+      </c>
+      <c r="I19" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" t="s">
+        <v>170</v>
+      </c>
+      <c r="K19" t="s">
+        <v>171</v>
+      </c>
+      <c r="L19" t="s">
+        <v>171</v>
+      </c>
+      <c r="M19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" t="s">
+        <v>101</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>84</v>
       </c>
-      <c r="G19">
-        <v>1</v>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" t="s">
+        <v>173</v>
+      </c>
+      <c r="J20" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" t="s">
+        <v>175</v>
+      </c>
+      <c r="L20" t="s">
+        <v>176</v>
+      </c>
+      <c r="M20" t="s">
+        <v>109</v>
+      </c>
+      <c r="N20" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" t="s">
+        <v>93</v>
+      </c>
+      <c r="K21" t="s">
+        <v>94</v>
+      </c>
+      <c r="L21" t="s">
+        <v>94</v>
+      </c>
+      <c r="M21" t="s">
+        <v>95</v>
+      </c>
+      <c r="N21" t="s">
+        <v>92</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>35</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1457,10 +2584,58 @@
       <c r="G22">
         <v>1</v>
       </c>
+      <c r="H22" t="s">
+        <v>177</v>
+      </c>
+      <c r="I22" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" t="s">
+        <v>179</v>
+      </c>
+      <c r="K22" t="s">
+        <v>180</v>
+      </c>
+      <c r="L22" t="s">
+        <v>180</v>
+      </c>
+      <c r="M22" t="s">
+        <v>109</v>
+      </c>
+      <c r="N22" t="s">
+        <v>101</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>71</v>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1475,38 +2650,134 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>181</v>
+      </c>
+      <c r="I23" t="s">
+        <v>182</v>
+      </c>
+      <c r="J23" t="s">
+        <v>183</v>
+      </c>
+      <c r="K23" t="s">
+        <v>184</v>
+      </c>
+      <c r="L23" t="s">
+        <v>184</v>
+      </c>
+      <c r="M23" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" t="s">
+        <v>101</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>87</v>
       </c>
-      <c r="G23">
-        <v>1</v>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>188</v>
+      </c>
+      <c r="I24" t="s">
+        <v>185</v>
+      </c>
+      <c r="J24" t="s">
+        <v>187</v>
+      </c>
+      <c r="K24" t="s">
+        <v>189</v>
+      </c>
+      <c r="L24" t="s">
+        <v>190</v>
+      </c>
+      <c r="M24" t="s">
+        <v>186</v>
+      </c>
+      <c r="N24" t="s">
+        <v>101</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24" t="s">
+        <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>37</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1526,10 +2797,58 @@
       <c r="G25">
         <v>1</v>
       </c>
+      <c r="H25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I25" t="s">
+        <v>193</v>
+      </c>
+      <c r="J25" t="s">
+        <v>194</v>
+      </c>
+      <c r="K25" t="s">
+        <v>195</v>
+      </c>
+      <c r="L25" t="s">
+        <v>196</v>
+      </c>
+      <c r="M25" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" t="s">
+        <v>197</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>72</v>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1544,66 +2863,210 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>198</v>
+      </c>
+      <c r="I26" t="s">
+        <v>199</v>
+      </c>
+      <c r="J26" t="s">
+        <v>200</v>
+      </c>
+      <c r="K26" t="s">
+        <v>201</v>
+      </c>
+      <c r="L26" t="s">
+        <v>201</v>
+      </c>
+      <c r="M26" t="s">
+        <v>109</v>
+      </c>
+      <c r="N26" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>89</v>
       </c>
-      <c r="G26">
-        <v>1</v>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>203</v>
+      </c>
+      <c r="I27" t="s">
+        <v>204</v>
+      </c>
+      <c r="J27" t="s">
+        <v>205</v>
+      </c>
+      <c r="K27" t="s">
+        <v>206</v>
+      </c>
+      <c r="L27" t="s">
+        <v>207</v>
+      </c>
+      <c r="M27" t="s">
+        <v>109</v>
+      </c>
+      <c r="N27" t="s">
+        <v>208</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27" t="s">
+        <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>90</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>91</v>
-      </c>
       <c r="G28">
         <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>210</v>
+      </c>
+      <c r="I28" t="s">
+        <v>211</v>
+      </c>
+      <c r="J28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K28" t="s">
+        <v>212</v>
+      </c>
+      <c r="L28" t="s">
+        <v>212</v>
+      </c>
+      <c r="M28">
+        <v>7</v>
+      </c>
+      <c r="N28" t="s">
+        <v>213</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>